<commit_message>
Updated water prices, and added xlsx prices for NG, elec, labor and water price calc
</commit_message>
<xml_diff>
--- a/input_fuel_pathway_data/labor_price_calcs.xlsx
+++ b/input_fuel_pathway_data/labor_price_calcs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danikamacdonell/Git/MIT_NavigaTE_inputs/input_fuel_pathway_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2889ACE-98BE-6044-98AE-97233EE43DE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD81CBB-7A50-8342-899C-2DC19B992BA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15560" activeTab="9" xr2:uid="{E23F0E55-3D1B-6848-8B97-956A5AEF3955}"/>
+    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15560" xr2:uid="{E23F0E55-3D1B-6848-8B97-956A5AEF3955}"/>
   </bookViews>
   <sheets>
     <sheet name="South Africa" sheetId="1" r:id="rId1"/>
@@ -867,8 +867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B19E802-EAE3-D348-9918-4E057FCB8B3A}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1026,8 +1026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37311316-4E35-BC49-A7F9-F074414CBB7D}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1659,6 +1659,7 @@
     <hyperlink ref="E3:E33" r:id="rId2" display="https://data.bls.gov/cgi-bin/cpicalc.pl?cost1=100.00&amp;year1=201601&amp;year2=202401" xr:uid="{F3011B54-FBFC-F54F-8ECF-0ADFD9901D91}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1667,7 +1668,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1718,7 +1719,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1769,7 +1770,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="A1:L2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1810,7 +1811,7 @@
       <c r="D2">
         <v>0.27227000000000001</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="7" t="s">
         <v>22</v>
       </c>
       <c r="F2" s="5">
@@ -1826,6 +1827,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{C5ECAF92-08BD-6C4B-B4FD-8AA3AA84EEB9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -1836,7 +1840,7 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1953,7 +1957,7 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2095,7 +2099,7 @@
   <dimension ref="A1:L1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="A1:L14"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2460,7 +2464,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2861,7 +2865,8 @@
       </c>
       <c r="G2" s="11"/>
       <c r="H2" s="6">
-        <v>10.0113228</v>
+        <f>A2*D2/L2</f>
+        <v>8.933047115384614</v>
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
@@ -2875,5 +2880,6 @@
     <hyperlink ref="C2" r:id="rId1" xr:uid="{BAE13540-8FA8-9049-B4EB-11FC397DCA20}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>